<commit_message>
ALs statements toegevoegd aan onvolledige_datum, completer maken steps implementatie, verschillende andere correcties
</commit_message>
<xml_diff>
--- a/features/brp_ingeschrevenpersonen.xlsx
+++ b/features/brp_ingeschrevenpersonen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Sites/VNG-sandbox/BRP/v1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/GitHub/Bevragingen-ingeschreven-personen/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDF4E89-BE10-6B44-A34F-D7234B282723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E0BFEF-E5BC-0C4E-8254-C263C311338A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="brp_ingeschrevenpersoon" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4087" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4214" uniqueCount="342">
   <si>
     <t>id</t>
   </si>
@@ -1000,6 +1000,57 @@
   </si>
   <si>
     <t>BI0518</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>indicatie_onjuist</t>
+  </si>
+  <si>
+    <t>Niet</t>
+  </si>
+  <si>
+    <t>Luik</t>
+  </si>
+  <si>
+    <t>33809a77-390a-4acd-9598-6833888495a9</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Leonel</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>6e0b6bc4-3344-4ec1-b87c-37099e48d4fe</t>
+  </si>
+  <si>
+    <t>906fd71b-ab43-4f9d-852a-9898ac8da836</t>
+  </si>
+  <si>
+    <t>c66674be-5789-4ede-9066-b85d32520d93</t>
+  </si>
+  <si>
+    <t>Baba</t>
+  </si>
+  <si>
+    <t>Riyad</t>
+  </si>
+  <si>
+    <t>8a328c17-3305-4a8b-938b-52581f7ebeda</t>
+  </si>
+  <si>
+    <t>14f15ad4-5836-419c-a578-a450a61920b6</t>
+  </si>
+  <si>
+    <t>Jesse</t>
   </si>
 </sst>
 </file>
@@ -1844,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO54"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10307,8 +10358,8 @@
       <c r="AR42" t="s">
         <v>81</v>
       </c>
-      <c r="AS42">
-        <v>19830526</v>
+      <c r="AS42" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="AT42">
         <v>6030</v>
@@ -13956,10 +14007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13967,7 +14018,7 @@
     <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -14025,8 +14076,11 @@
       <c r="S1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -14084,8 +14138,11 @@
       <c r="S2">
         <v>6030</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -14143,8 +14200,11 @@
       <c r="S3">
         <v>6030</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -14202,8 +14262,11 @@
       <c r="S4">
         <v>6030</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -14261,8 +14324,11 @@
       <c r="S5">
         <v>6030</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>217</v>
       </c>
@@ -14320,8 +14386,11 @@
       <c r="S6">
         <v>6030</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -14379,8 +14448,11 @@
       <c r="S7">
         <v>6030</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -14438,8 +14510,11 @@
       <c r="S8">
         <v>6030</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -14497,8 +14572,11 @@
       <c r="S9">
         <v>6030</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -14556,8 +14634,11 @@
       <c r="S10">
         <v>6030</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>210</v>
       </c>
@@ -14615,8 +14696,11 @@
       <c r="S11">
         <v>6030</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>209</v>
       </c>
@@ -14674,8 +14758,11 @@
       <c r="S12">
         <v>6030</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -14733,8 +14820,11 @@
       <c r="S13">
         <v>6030</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>207</v>
       </c>
@@ -14792,8 +14882,11 @@
       <c r="S14">
         <v>6030</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>206</v>
       </c>
@@ -14851,8 +14944,11 @@
       <c r="S15">
         <v>6030</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>205</v>
       </c>
@@ -14910,8 +15006,11 @@
       <c r="S16">
         <v>6030</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -14969,8 +15068,11 @@
       <c r="S17">
         <v>6030</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>203</v>
       </c>
@@ -15028,8 +15130,11 @@
       <c r="S18">
         <v>6030</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>202</v>
       </c>
@@ -15087,8 +15192,11 @@
       <c r="S19">
         <v>6030</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>200</v>
       </c>
@@ -15146,8 +15254,11 @@
       <c r="S20">
         <v>6030</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -15205,8 +15316,11 @@
       <c r="S21">
         <v>6030</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>197</v>
       </c>
@@ -15264,8 +15378,11 @@
       <c r="S22">
         <v>6030</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -15323,8 +15440,11 @@
       <c r="S23">
         <v>6030</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>193</v>
       </c>
@@ -15382,8 +15502,11 @@
       <c r="S24">
         <v>6030</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>191</v>
       </c>
@@ -15441,8 +15564,11 @@
       <c r="S25">
         <v>6030</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>190</v>
       </c>
@@ -15500,8 +15626,11 @@
       <c r="S26">
         <v>6030</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>188</v>
       </c>
@@ -15559,8 +15688,11 @@
       <c r="S27">
         <v>6030</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>186</v>
       </c>
@@ -15618,8 +15750,11 @@
       <c r="S28">
         <v>6030</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>185</v>
       </c>
@@ -15677,8 +15812,11 @@
       <c r="S29">
         <v>6030</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -15736,8 +15874,11 @@
       <c r="S30">
         <v>6030</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -15795,8 +15936,11 @@
       <c r="S31">
         <v>6030</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>180</v>
       </c>
@@ -15854,8 +15998,11 @@
       <c r="S32">
         <v>6043</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>177</v>
       </c>
@@ -15913,8 +16060,11 @@
       <c r="S33">
         <v>6043</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -15972,8 +16122,11 @@
       <c r="S34">
         <v>6023</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -16031,8 +16184,11 @@
       <c r="S35">
         <v>6030</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>299</v>
       </c>
@@ -16090,8 +16246,11 @@
       <c r="S36">
         <v>6030</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>300</v>
       </c>
@@ -16148,6 +16307,133 @@
       </c>
       <c r="S37">
         <v>6030</v>
+      </c>
+      <c r="T37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>329</v>
+      </c>
+      <c r="B38">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" t="s">
+        <v>327</v>
+      </c>
+      <c r="H38" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" t="s">
+        <v>328</v>
+      </c>
+      <c r="K38">
+        <v>19911111</v>
+      </c>
+      <c r="L38">
+        <v>5010</v>
+      </c>
+      <c r="M38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N38" t="s">
+        <v>59</v>
+      </c>
+      <c r="O38" t="s">
+        <v>59</v>
+      </c>
+      <c r="P38" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>84</v>
+      </c>
+      <c r="R38">
+        <v>20110426</v>
+      </c>
+      <c r="S38">
+        <v>6030</v>
+      </c>
+      <c r="T38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>334</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>332</v>
+      </c>
+      <c r="G39" t="s">
+        <v>330</v>
+      </c>
+      <c r="H39" t="s">
+        <v>331</v>
+      </c>
+      <c r="I39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" t="s">
+        <v>333</v>
+      </c>
+      <c r="K39">
+        <v>19790730</v>
+      </c>
+      <c r="L39">
+        <v>6037</v>
+      </c>
+      <c r="M39" t="s">
+        <v>66</v>
+      </c>
+      <c r="N39" t="s">
+        <v>89</v>
+      </c>
+      <c r="O39">
+        <v>20060714</v>
+      </c>
+      <c r="P39">
+        <v>6030</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>66</v>
+      </c>
+      <c r="R39">
+        <v>20050126</v>
+      </c>
+      <c r="S39">
+        <v>6030</v>
+      </c>
+      <c r="T39" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -16158,10 +16444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B13" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16171,7 +16457,7 @@
     <col min="11" max="11" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -16211,8 +16497,11 @@
       <c r="M1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>243</v>
       </c>
@@ -16252,8 +16541,11 @@
       <c r="M2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>251</v>
       </c>
@@ -16293,8 +16585,11 @@
       <c r="M3">
         <v>5002</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>257</v>
       </c>
@@ -16334,8 +16629,11 @@
       <c r="M4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>258</v>
       </c>
@@ -16375,8 +16673,11 @@
       <c r="M5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -16416,8 +16717,11 @@
       <c r="M6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>268</v>
       </c>
@@ -16457,8 +16761,11 @@
       <c r="M7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>269</v>
       </c>
@@ -16498,8 +16805,11 @@
       <c r="M8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -16539,8 +16849,11 @@
       <c r="M9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>275</v>
       </c>
@@ -16580,8 +16893,11 @@
       <c r="M10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>309</v>
       </c>
@@ -16621,8 +16937,11 @@
       <c r="M11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>310</v>
       </c>
@@ -16662,8 +16981,11 @@
       <c r="M12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>311</v>
       </c>
@@ -16702,6 +17024,94 @@
       </c>
       <c r="M13" t="s">
         <v>59</v>
+      </c>
+      <c r="N13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>335</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>19830526</v>
+      </c>
+      <c r="G14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" t="s">
+        <v>337</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" t="s">
+        <v>338</v>
+      </c>
+      <c r="L14">
+        <v>19560904</v>
+      </c>
+      <c r="M14">
+        <v>5018</v>
+      </c>
+      <c r="N14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>999999370</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>19830526</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -16712,10 +17122,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16726,7 +17136,7 @@
     <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -16763,8 +17173,11 @@
       <c r="L1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>252</v>
       </c>
@@ -16801,8 +17214,11 @@
       <c r="L2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>253</v>
       </c>
@@ -16839,8 +17255,11 @@
       <c r="L3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -16877,8 +17296,11 @@
       <c r="L4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>260</v>
       </c>
@@ -16915,8 +17337,11 @@
       <c r="L5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>263</v>
       </c>
@@ -16953,8 +17378,11 @@
       <c r="L6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>264</v>
       </c>
@@ -16991,8 +17419,11 @@
       <c r="L7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -17029,8 +17460,11 @@
       <c r="L8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>266</v>
       </c>
@@ -17067,8 +17501,11 @@
       <c r="L9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>273</v>
       </c>
@@ -17105,8 +17542,11 @@
       <c r="L10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -17142,6 +17582,91 @@
       </c>
       <c r="L11">
         <v>6043</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B12">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12">
+        <v>20190117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>341</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K12">
+        <v>20190114</v>
+      </c>
+      <c r="L12">
+        <v>6043</v>
+      </c>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>999999023</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13">
+        <v>19830526</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -17154,7 +17679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7F0AE2-82CE-2540-9560-8B970AA2C400}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>